<commit_message>
update change to service and change js 1 file
</commit_message>
<xml_diff>
--- a/public/file_excel/tuyensinh/form-export-data-tuyen-sinh.xlsx
+++ b/public/file_excel/tuyensinh/form-export-data-tuyen-sinh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\du-an-ldtbxh-hn\public\file_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\du-an-ldtbxh-hn\public\file_excel\tuyensinh\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>TT</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trường </t>
   </si>
 </sst>
 </file>
@@ -300,13 +297,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -315,13 +315,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -617,304 +614,304 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
     </row>
     <row r="2" spans="1:37" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="3" t="s">
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="3"/>
-      <c r="AJ3" s="3"/>
-      <c r="AK3" s="3"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="8" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3" t="s">
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3" t="s">
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AE4" s="6" t="s">
+      <c r="AE4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="3" t="s">
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AI4" s="10" t="s">
+      <c r="AI4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="3" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="4" t="s">
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="V5" s="4" t="s">
+      <c r="V5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="W5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="X5" s="6" t="s">
+      <c r="X5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="4" t="s">
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AC5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="8" t="s">
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AF5" s="8" t="s">
+      <c r="AF5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AG5" s="8" t="s">
+      <c r="AG5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="8" t="s">
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AJ5" s="8" t="s">
+      <c r="AJ5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AK5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:37" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="3"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="6"/>
       <c r="R6" s="1" t="s">
         <v>19</v>
       </c>
@@ -924,9 +921,9 @@
       <c r="T6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="3"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="6"/>
       <c r="X6" s="1" t="s">
         <v>19</v>
       </c>
@@ -939,27 +936,52 @@
       <c r="AA6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
-      <c r="AK6" s="8"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="K3:K6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="L3:L6"/>
+    <mergeCell ref="M2:AK2"/>
+    <mergeCell ref="M3:M6"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:AK3"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="I3:I6"/>
     <mergeCell ref="AJ5:AJ6"/>
     <mergeCell ref="AK5:AK6"/>
     <mergeCell ref="A1:AK1"/>
@@ -976,33 +998,6 @@
     <mergeCell ref="Q5:Q6"/>
     <mergeCell ref="R5:T5"/>
     <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="L3:L6"/>
-    <mergeCell ref="M2:AK2"/>
-    <mergeCell ref="M3:M6"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:AK3"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="O4:O6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="Q4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="I3:I6"/>
-    <mergeCell ref="K3:K6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="J3:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>